<commit_message>
Update to functions, vignettes
</commit_message>
<xml_diff>
--- a/data-raw/microwaveAH_adjMat_20230629.xlsx
+++ b/data-raw/microwaveAH_adjMat_20230629.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbedinge\Documents\GitHub\AHgen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbedinge\Documents\GitHub\AHgen\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="39">
   <si>
     <t>To cook food</t>
   </si>
@@ -97,6 +97,45 @@
   </si>
   <si>
     <t>Node</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>levelName_full</t>
+  </si>
+  <si>
+    <t>levelName</t>
+  </si>
+  <si>
+    <t>Functional purposes</t>
+  </si>
+  <si>
+    <t>Purposes</t>
+  </si>
+  <si>
+    <t>Values and priority measures</t>
+  </si>
+  <si>
+    <t>Outcomes</t>
+  </si>
+  <si>
+    <t>Generalised functions</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Object-related processes</t>
+  </si>
+  <si>
+    <t>Processes</t>
+  </si>
+  <si>
+    <t>Physical objects</t>
+  </si>
+  <si>
+    <t>Resources</t>
   </si>
 </sst>
 </file>
@@ -252,7 +291,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -438,8 +477,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -569,6 +614,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -614,7 +674,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -631,6 +691,11 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1063,8 +1128,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Z26" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A1:Z26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="D1:AC26" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="D1:AC26">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1327,122 +1392,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z26"/>
+  <dimension ref="A1:AC26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.75" style="2" customWidth="1"/>
-    <col min="3" max="26" width="2.75" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.75" style="2" customWidth="1"/>
+    <col min="6" max="29" width="2.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="3" customFormat="1" ht="180" customHeight="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:29" s="3" customFormat="1" ht="180" customHeight="1" thickBot="1">
+      <c r="A1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="12" customHeight="1">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:29" ht="12" customHeight="1">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8">
-        <v>1</v>
-      </c>
-      <c r="D2" s="8">
-        <v>1</v>
-      </c>
-      <c r="E2" s="8">
-        <v>1</v>
-      </c>
+      <c r="E2" s="7"/>
       <c r="F2" s="8">
         <v>1</v>
       </c>
       <c r="G2" s="8">
         <v>1</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
+      <c r="H2" s="8">
+        <v>1</v>
+      </c>
+      <c r="I2" s="8">
+        <v>1</v>
+      </c>
+      <c r="J2" s="8">
+        <v>1</v>
+      </c>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
@@ -1459,34 +1539,43 @@
       <c r="X2" s="8"/>
       <c r="Y2" s="8"/>
       <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
     </row>
-    <row r="3" spans="1:26" ht="12" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+    <row r="3" spans="1:29" ht="12" customHeight="1">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="8">
-        <v>1</v>
-      </c>
-      <c r="I3" s="8">
-        <v>1</v>
-      </c>
-      <c r="J3" s="8">
-        <v>1</v>
-      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
       <c r="K3" s="8">
         <v>1</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
+      <c r="L3" s="8">
+        <v>1</v>
+      </c>
+      <c r="M3" s="8">
+        <v>1</v>
+      </c>
+      <c r="N3" s="8">
+        <v>1</v>
+      </c>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
@@ -1499,29 +1588,38 @@
       <c r="X3" s="8"/>
       <c r="Y3" s="8"/>
       <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
     </row>
-    <row r="4" spans="1:26" ht="12" customHeight="1">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:29" ht="12" customHeight="1">
+      <c r="A4" s="11">
         <v>2</v>
       </c>
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
+      <c r="B4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="9">
+        <v>1</v>
+      </c>
       <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="G4" s="7"/>
       <c r="H4" s="8"/>
-      <c r="I4" s="8">
-        <v>1</v>
-      </c>
-      <c r="J4" s="8">
-        <v>1</v>
-      </c>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
       <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
+      <c r="L4" s="8">
+        <v>1</v>
+      </c>
+      <c r="M4" s="8">
+        <v>1</v>
+      </c>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
       <c r="P4" s="8"/>
@@ -1535,30 +1633,39 @@
       <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
     </row>
-    <row r="5" spans="1:26" ht="12" customHeight="1">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:29" ht="12" customHeight="1">
+      <c r="A5" s="10">
+        <v>2</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="9">
-        <v>1</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="9">
+        <v>1</v>
+      </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="H5" s="7"/>
       <c r="I5" s="8"/>
-      <c r="J5" s="8">
-        <v>1</v>
-      </c>
-      <c r="K5" s="8">
-        <v>1</v>
-      </c>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
       <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
+      <c r="M5" s="8">
+        <v>1</v>
+      </c>
+      <c r="N5" s="8">
+        <v>1</v>
+      </c>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
@@ -1571,32 +1678,41 @@
       <c r="X5" s="8"/>
       <c r="Y5" s="8"/>
       <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="8"/>
     </row>
-    <row r="6" spans="1:26" ht="12" customHeight="1">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:29" ht="12" customHeight="1">
+      <c r="A6" s="11">
+        <v>2</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9">
-        <v>1</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="7"/>
+      <c r="E6" s="9">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="8">
-        <v>1</v>
-      </c>
-      <c r="J6" s="8">
-        <v>1</v>
-      </c>
-      <c r="K6" s="8">
-        <v>1</v>
-      </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8">
+        <v>1</v>
+      </c>
+      <c r="M6" s="8">
+        <v>1</v>
+      </c>
+      <c r="N6" s="8">
+        <v>1</v>
+      </c>
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
@@ -1609,32 +1725,41 @@
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
     </row>
-    <row r="7" spans="1:26" ht="12" customHeight="1">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:29" ht="12" customHeight="1">
+      <c r="A7" s="10">
+        <v>2</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="9">
-        <v>1</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="E7" s="9">
+        <v>1</v>
+      </c>
       <c r="F7" s="8"/>
-      <c r="G7" s="7"/>
+      <c r="G7" s="8"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="8">
-        <v>1</v>
-      </c>
-      <c r="J7" s="8">
-        <v>1</v>
-      </c>
-      <c r="K7" s="8">
-        <v>1</v>
-      </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8">
+        <v>1</v>
+      </c>
+      <c r="M7" s="8">
+        <v>1</v>
+      </c>
+      <c r="N7" s="8">
+        <v>1</v>
+      </c>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
@@ -1647,55 +1772,69 @@
       <c r="X7" s="8"/>
       <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
     </row>
-    <row r="8" spans="1:26" ht="12" customHeight="1">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:29" ht="12" customHeight="1">
+      <c r="A8" s="11">
+        <v>3</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
       <c r="G8" s="8"/>
-      <c r="H8" s="7"/>
+      <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8">
-        <v>1</v>
-      </c>
+      <c r="K8" s="7"/>
+      <c r="L8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
+      <c r="O8" s="8">
+        <v>1</v>
+      </c>
       <c r="P8" s="8"/>
-      <c r="Q8" s="8">
-        <v>1</v>
-      </c>
+      <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
+      <c r="T8" s="8">
+        <v>1</v>
+      </c>
       <c r="U8" s="8"/>
       <c r="V8" s="8"/>
       <c r="W8" s="8"/>
       <c r="X8" s="8"/>
       <c r="Y8" s="8"/>
       <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
     </row>
-    <row r="9" spans="1:26" ht="12" customHeight="1">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:29" ht="12" customHeight="1">
+      <c r="A9" s="10">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="8">
-        <v>1</v>
-      </c>
-      <c r="D9" s="8">
-        <v>1</v>
-      </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="8">
         <v>1</v>
       </c>
@@ -1703,64 +1842,77 @@
         <v>1</v>
       </c>
       <c r="H9" s="8"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="8"/>
+      <c r="I9" s="8">
+        <v>1</v>
+      </c>
+      <c r="J9" s="8">
+        <v>1</v>
+      </c>
       <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8">
-        <v>1</v>
-      </c>
+      <c r="L9" s="7"/>
+      <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
+      <c r="P9" s="8">
+        <v>1</v>
+      </c>
       <c r="Q9" s="8"/>
-      <c r="R9" s="8">
-        <v>1</v>
-      </c>
+      <c r="R9" s="8"/>
       <c r="S9" s="8"/>
       <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
+      <c r="U9" s="8">
+        <v>1</v>
+      </c>
       <c r="V9" s="8"/>
       <c r="W9" s="8"/>
       <c r="X9" s="8"/>
       <c r="Y9" s="8"/>
       <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
     </row>
-    <row r="10" spans="1:26" ht="12" customHeight="1">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:29" ht="12" customHeight="1">
+      <c r="A10" s="11">
+        <v>3</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="8">
-        <v>1</v>
-      </c>
-      <c r="D10" s="8">
-        <v>1</v>
-      </c>
-      <c r="E10" s="8">
-        <v>1</v>
-      </c>
+      <c r="E10" s="9"/>
       <c r="F10" s="8">
         <v>1</v>
       </c>
       <c r="G10" s="8">
         <v>1</v>
       </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="7"/>
+      <c r="H10" s="8">
+        <v>1</v>
+      </c>
+      <c r="I10" s="8">
+        <v>1</v>
+      </c>
+      <c r="J10" s="8">
+        <v>1</v>
+      </c>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8">
-        <v>1</v>
-      </c>
-      <c r="O10" s="8">
-        <v>1</v>
-      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
       <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
+      <c r="Q10" s="8">
+        <v>1</v>
+      </c>
+      <c r="R10" s="8">
+        <v>1</v>
+      </c>
       <c r="S10" s="8"/>
       <c r="T10" s="8"/>
       <c r="U10" s="8"/>
@@ -1769,41 +1921,50 @@
       <c r="X10" s="8"/>
       <c r="Y10" s="8"/>
       <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="8"/>
     </row>
-    <row r="11" spans="1:26" ht="12" customHeight="1">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:29" ht="12" customHeight="1">
+      <c r="A11" s="10">
+        <v>3</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="8">
-        <v>1</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8">
-        <v>1</v>
-      </c>
+      <c r="E11" s="9"/>
       <c r="F11" s="8">
         <v>1</v>
       </c>
-      <c r="G11" s="8">
-        <v>1</v>
-      </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8">
+        <v>1</v>
+      </c>
+      <c r="I11" s="8">
+        <v>1</v>
+      </c>
+      <c r="J11" s="8">
+        <v>1</v>
+      </c>
+      <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
-      <c r="N11" s="8">
-        <v>1</v>
-      </c>
+      <c r="N11" s="7"/>
       <c r="O11" s="8"/>
-      <c r="P11" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8">
+        <v>1</v>
+      </c>
       <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
+      <c r="S11" s="8">
+        <v>1</v>
+      </c>
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
@@ -1811,289 +1972,370 @@
       <c r="X11" s="8"/>
       <c r="Y11" s="8"/>
       <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="8"/>
     </row>
-    <row r="12" spans="1:26" ht="12" customHeight="1">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:29" ht="12" customHeight="1">
+      <c r="A12" s="11">
+        <v>4</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="E12" s="9"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="8">
-        <v>1</v>
-      </c>
+      <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="7"/>
+      <c r="K12" s="8">
+        <v>1</v>
+      </c>
+      <c r="L12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
+      <c r="O12" s="7"/>
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
-      <c r="S12" s="8">
-        <v>1</v>
-      </c>
+      <c r="S12" s="8"/>
       <c r="T12" s="8"/>
       <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
+      <c r="V12" s="8">
+        <v>1</v>
+      </c>
       <c r="W12" s="8"/>
       <c r="X12" s="8"/>
       <c r="Y12" s="8"/>
       <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="8"/>
+      <c r="AC12" s="8"/>
     </row>
-    <row r="13" spans="1:26" ht="12" customHeight="1">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:29" ht="12" customHeight="1">
+      <c r="A13" s="10">
+        <v>4</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="E13" s="9"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="8">
-        <v>1</v>
-      </c>
+      <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="7"/>
+      <c r="L13" s="8">
+        <v>1</v>
+      </c>
+      <c r="M13" s="8"/>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
+      <c r="P13" s="7"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
       <c r="T13" s="8"/>
-      <c r="U13" s="8">
-        <v>1</v>
-      </c>
+      <c r="U13" s="8"/>
       <c r="V13" s="8"/>
       <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
+      <c r="X13" s="8">
+        <v>1</v>
+      </c>
       <c r="Y13" s="8"/>
       <c r="Z13" s="8"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
+      <c r="AC13" s="8"/>
     </row>
-    <row r="14" spans="1:26" ht="12" customHeight="1">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:29" ht="12" customHeight="1">
+      <c r="A14" s="11">
+        <v>4</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="8">
-        <v>1</v>
-      </c>
-      <c r="K14" s="8">
-        <v>1</v>
-      </c>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
       <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="7"/>
+      <c r="M14" s="8">
+        <v>1</v>
+      </c>
+      <c r="N14" s="8">
+        <v>1</v>
+      </c>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
+      <c r="Q14" s="7"/>
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
-      <c r="T14" s="8">
-        <v>1</v>
-      </c>
+      <c r="T14" s="8"/>
       <c r="U14" s="8"/>
       <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
+      <c r="W14" s="8">
+        <v>1</v>
+      </c>
       <c r="X14" s="8"/>
       <c r="Y14" s="8"/>
       <c r="Z14" s="8"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
+      <c r="AC14" s="8"/>
     </row>
-    <row r="15" spans="1:26" ht="12" customHeight="1">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:29" ht="12" customHeight="1">
+      <c r="A15" s="10">
+        <v>4</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="E15" s="9"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
-      <c r="J15" s="8">
-        <v>1</v>
-      </c>
+      <c r="J15" s="8"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
+      <c r="M15" s="8">
+        <v>1</v>
+      </c>
       <c r="N15" s="8"/>
-      <c r="O15" s="7"/>
+      <c r="O15" s="8"/>
       <c r="P15" s="8"/>
       <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
+      <c r="R15" s="7"/>
       <c r="S15" s="8"/>
       <c r="T15" s="8"/>
       <c r="U15" s="8"/>
-      <c r="V15" s="8">
-        <v>1</v>
-      </c>
+      <c r="V15" s="8"/>
       <c r="W15" s="8"/>
       <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
+      <c r="Y15" s="8">
+        <v>1</v>
+      </c>
       <c r="Z15" s="8"/>
+      <c r="AA15" s="8"/>
+      <c r="AB15" s="8"/>
+      <c r="AC15" s="8"/>
     </row>
-    <row r="16" spans="1:26" ht="12" customHeight="1">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:29" ht="12" customHeight="1">
+      <c r="A16" s="11">
+        <v>4</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="E16" s="9"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
-      <c r="K16" s="8">
-        <v>1</v>
-      </c>
+      <c r="K16" s="8"/>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
+      <c r="N16" s="8">
+        <v>1</v>
+      </c>
       <c r="O16" s="8"/>
-      <c r="P16" s="7"/>
+      <c r="P16" s="8"/>
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
+      <c r="S16" s="7"/>
       <c r="T16" s="8"/>
       <c r="U16" s="8"/>
       <c r="V16" s="8"/>
-      <c r="W16" s="8">
-        <v>1</v>
-      </c>
-      <c r="X16" s="8">
-        <v>1</v>
-      </c>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
       <c r="Y16" s="8"/>
-      <c r="Z16" s="8"/>
+      <c r="Z16" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="8">
+        <v>1</v>
+      </c>
+      <c r="AB16" s="8"/>
+      <c r="AC16" s="8"/>
     </row>
-    <row r="17" spans="1:26" ht="12" customHeight="1">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:29" ht="12" customHeight="1">
+      <c r="A17" s="10">
+        <v>4</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="E17" s="9"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
-      <c r="H17" s="8">
-        <v>1</v>
-      </c>
+      <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
+      <c r="K17" s="8">
+        <v>1</v>
+      </c>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
-      <c r="Q17" s="7"/>
+      <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
+      <c r="T17" s="7"/>
       <c r="U17" s="8"/>
       <c r="V17" s="8"/>
       <c r="W17" s="8"/>
       <c r="X17" s="8"/>
-      <c r="Y17" s="8">
-        <v>1</v>
-      </c>
+      <c r="Y17" s="8"/>
       <c r="Z17" s="8"/>
+      <c r="AA17" s="8"/>
+      <c r="AB17" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC17" s="8"/>
     </row>
-    <row r="18" spans="1:26" ht="12" customHeight="1">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:29" ht="12" customHeight="1">
+      <c r="A18" s="11">
+        <v>4</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="E18" s="9"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
-      <c r="I18" s="8">
-        <v>1</v>
-      </c>
+      <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
+      <c r="L18" s="8">
+        <v>1</v>
+      </c>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
-      <c r="R18" s="7"/>
+      <c r="R18" s="8"/>
       <c r="S18" s="8"/>
       <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
+      <c r="U18" s="7"/>
       <c r="V18" s="8"/>
       <c r="W18" s="8"/>
       <c r="X18" s="8"/>
       <c r="Y18" s="8"/>
-      <c r="Z18" s="8">
+      <c r="Z18" s="8"/>
+      <c r="AA18" s="8"/>
+      <c r="AB18" s="8"/>
+      <c r="AC18" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="12" customHeight="1">
-      <c r="A19" s="6" t="s">
+    <row r="19" spans="1:29" ht="12" customHeight="1">
+      <c r="A19" s="10">
+        <v>5</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="E19" s="9"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
-      <c r="L19" s="8">
-        <v>1</v>
-      </c>
+      <c r="L19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
+      <c r="O19" s="8">
+        <v>1</v>
+      </c>
       <c r="P19" s="8"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
-      <c r="S19" s="7"/>
+      <c r="S19" s="8"/>
       <c r="T19" s="8"/>
       <c r="U19" s="8"/>
-      <c r="V19" s="8"/>
+      <c r="V19" s="7"/>
       <c r="W19" s="8"/>
       <c r="X19" s="8"/>
       <c r="Y19" s="8"/>
       <c r="Z19" s="8"/>
+      <c r="AA19" s="8"/>
+      <c r="AB19" s="8"/>
+      <c r="AC19" s="8"/>
     </row>
-    <row r="20" spans="1:26" ht="12" customHeight="1">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:29" ht="12" customHeight="1">
+      <c r="A20" s="11">
+        <v>5</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="E20" s="9"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
@@ -2102,30 +2344,39 @@
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
-      <c r="N20" s="8">
-        <v>1</v>
-      </c>
+      <c r="N20" s="8"/>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
+      <c r="Q20" s="8">
+        <v>1</v>
+      </c>
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
-      <c r="T20" s="7"/>
+      <c r="T20" s="8"/>
       <c r="U20" s="8"/>
       <c r="V20" s="8"/>
-      <c r="W20" s="8"/>
+      <c r="W20" s="7"/>
       <c r="X20" s="8"/>
       <c r="Y20" s="8"/>
       <c r="Z20" s="8"/>
+      <c r="AA20" s="8"/>
+      <c r="AB20" s="8"/>
+      <c r="AC20" s="8"/>
     </row>
-    <row r="21" spans="1:26" ht="12" customHeight="1">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:29" ht="12" customHeight="1">
+      <c r="A21" s="10">
+        <v>5</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="E21" s="9"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -2133,31 +2384,40 @@
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
-      <c r="M21" s="8">
-        <v>1</v>
-      </c>
+      <c r="M21" s="8"/>
       <c r="N21" s="8"/>
       <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
+      <c r="P21" s="8">
+        <v>1</v>
+      </c>
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
       <c r="T21" s="8"/>
-      <c r="U21" s="7"/>
+      <c r="U21" s="8"/>
       <c r="V21" s="8"/>
       <c r="W21" s="8"/>
-      <c r="X21" s="8"/>
+      <c r="X21" s="7"/>
       <c r="Y21" s="8"/>
       <c r="Z21" s="8"/>
+      <c r="AA21" s="8"/>
+      <c r="AB21" s="8"/>
+      <c r="AC21" s="8"/>
     </row>
-    <row r="22" spans="1:26" ht="12" customHeight="1">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:29" ht="12" customHeight="1">
+      <c r="A22" s="11">
+        <v>5</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -2167,29 +2427,38 @@
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
-      <c r="O22" s="8">
-        <v>1</v>
-      </c>
+      <c r="O22" s="8"/>
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
+      <c r="R22" s="8">
+        <v>1</v>
+      </c>
       <c r="S22" s="8"/>
       <c r="T22" s="8"/>
       <c r="U22" s="8"/>
-      <c r="V22" s="7"/>
+      <c r="V22" s="8"/>
       <c r="W22" s="8"/>
       <c r="X22" s="8"/>
-      <c r="Y22" s="8"/>
+      <c r="Y22" s="7"/>
       <c r="Z22" s="8"/>
+      <c r="AA22" s="8"/>
+      <c r="AB22" s="8"/>
+      <c r="AC22" s="8"/>
     </row>
-    <row r="23" spans="1:26" ht="12" customHeight="1">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:29" ht="12" customHeight="1">
+      <c r="A23" s="10">
+        <v>5</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="E23" s="9"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -2200,28 +2469,37 @@
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
       <c r="O23" s="8"/>
-      <c r="P23" s="8">
-        <v>1</v>
-      </c>
+      <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
+      <c r="S23" s="8">
+        <v>1</v>
+      </c>
       <c r="T23" s="8"/>
       <c r="U23" s="8"/>
       <c r="V23" s="8"/>
-      <c r="W23" s="7"/>
+      <c r="W23" s="8"/>
       <c r="X23" s="8"/>
       <c r="Y23" s="8"/>
-      <c r="Z23" s="8"/>
+      <c r="Z23" s="7"/>
+      <c r="AA23" s="8"/>
+      <c r="AB23" s="8"/>
+      <c r="AC23" s="8"/>
     </row>
-    <row r="24" spans="1:26" ht="12" customHeight="1">
-      <c r="A24" s="6" t="s">
+    <row r="24" spans="1:29" ht="12" customHeight="1">
+      <c r="A24" s="11">
+        <v>5</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
@@ -2232,28 +2510,37 @@
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
-      <c r="P24" s="8">
-        <v>1</v>
-      </c>
+      <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
+      <c r="S24" s="8">
+        <v>1</v>
+      </c>
       <c r="T24" s="8"/>
       <c r="U24" s="8"/>
       <c r="V24" s="8"/>
       <c r="W24" s="8"/>
-      <c r="X24" s="7"/>
+      <c r="X24" s="8"/>
       <c r="Y24" s="8"/>
       <c r="Z24" s="8"/>
+      <c r="AA24" s="7"/>
+      <c r="AB24" s="8"/>
+      <c r="AC24" s="8"/>
     </row>
-    <row r="25" spans="1:26" ht="12" customHeight="1">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:29" ht="12" customHeight="1">
+      <c r="A25" s="10">
+        <v>5</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
+      <c r="E25" s="9"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
@@ -2265,27 +2552,36 @@
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
-      <c r="Q25" s="8">
-        <v>1</v>
-      </c>
+      <c r="Q25" s="8"/>
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
+      <c r="T25" s="8">
+        <v>1</v>
+      </c>
       <c r="U25" s="8"/>
       <c r="V25" s="8"/>
       <c r="W25" s="8"/>
       <c r="X25" s="8"/>
-      <c r="Y25" s="7"/>
+      <c r="Y25" s="8"/>
       <c r="Z25" s="8"/>
+      <c r="AA25" s="8"/>
+      <c r="AB25" s="7"/>
+      <c r="AC25" s="8"/>
     </row>
-    <row r="26" spans="1:26" ht="12" customHeight="1">
-      <c r="A26" s="6" t="s">
+    <row r="26" spans="1:29" ht="12" customHeight="1">
+      <c r="A26" s="11">
+        <v>5</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+      <c r="E26" s="9"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
@@ -2298,17 +2594,20 @@
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
       <c r="Q26" s="8"/>
-      <c r="R26" s="8">
-        <v>1</v>
-      </c>
+      <c r="R26" s="8"/>
       <c r="S26" s="8"/>
       <c r="T26" s="8"/>
-      <c r="U26" s="8"/>
+      <c r="U26" s="8">
+        <v>1</v>
+      </c>
       <c r="V26" s="8"/>
       <c r="W26" s="8"/>
       <c r="X26" s="8"/>
       <c r="Y26" s="8"/>
-      <c r="Z26" s="7"/>
+      <c r="Z26" s="8"/>
+      <c r="AA26" s="8"/>
+      <c r="AB26" s="8"/>
+      <c r="AC26" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>